<commit_message>
Data entry for gadget and crime tables
</commit_message>
<xml_diff>
--- a/sql/SuperVillainDB.xlsx
+++ b/sql/SuperVillainDB.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="aliases" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="crime" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="gadget" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="gadget_crime" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="180">
   <si>
     <t>name</t>
   </si>
@@ -296,10 +297,265 @@
     <t>description</t>
   </si>
   <si>
+    <t>Attempted theft of the Mammoth of Moldavia - Filled with priceless stamps</t>
+  </si>
+  <si>
+    <t>Ransoming the city of Gotham for $1,000,000 by planting a bomb inside Gotham City Hall of Fame</t>
+  </si>
+  <si>
+    <t>Kidnapping of Robin - The Boy Wonder</t>
+  </si>
+  <si>
+    <t>Escape from Gotham State Penitentiary</t>
+  </si>
+  <si>
+    <t>Robbery of patrons of Gotham Opera</t>
+  </si>
+  <si>
+    <t>Theft of priceless African masks</t>
+  </si>
+  <si>
+    <t>Theft of anwer key to Nationwide Pre-College Exam</t>
+  </si>
+  <si>
+    <t>Framing of Woodrow Wilson High School Basketball for cheating on exams</t>
+  </si>
+  <si>
+    <t>Kidnapping of the Maharaja of Nimpah</t>
+  </si>
+  <si>
+    <t>Theft of golden cat statue from Gotham Museum</t>
+  </si>
+  <si>
+    <t>Attempted theft of jewels belonging to socialite Sophia Starr</t>
+  </si>
+  <si>
+    <t>Theft of wedding gifts</t>
+  </si>
+  <si>
+    <t>Kidnapping of Barbara Gordon</t>
+  </si>
+  <si>
+    <t>Theft of Gotham City Charter</t>
+  </si>
+  <si>
+    <t>Kidnapping of Bruce Wayne</t>
+  </si>
+  <si>
+    <t>Theft of the Star of Cahmere (most valuable diamond in Gotham City)</t>
+  </si>
+  <si>
+    <t>Theft of the Ghiaccio Circulo (world's most valuable diamond)</t>
+  </si>
+  <si>
+    <t>Kidnapping of Paul Diamante (Pitcher for the Gotham City Eagles)</t>
+  </si>
+  <si>
+    <t>Melting Gothamn City Ice Rink</t>
+  </si>
+  <si>
+    <t>Robbery of movie theatre patrons</t>
+  </si>
+  <si>
+    <t>Looting Gotham Drugtstore</t>
+  </si>
+  <si>
+    <t>Takeover of Gotham State Penitentiary</t>
+  </si>
+  <si>
+    <t>Attempted theft of atomic powered Cesium Clock</t>
+  </si>
+  <si>
+    <t>Robbery at Harry Hummert Jewelry Shop</t>
+  </si>
+  <si>
+    <t>Attempted theft of rare time-related painting</t>
+  </si>
+  <si>
+    <t>Attempted theft of Batman's cowl</t>
+  </si>
+  <si>
+    <t>Kidnapping of jury responsible for convicting him</t>
+  </si>
+  <si>
+    <t>Ransoming of collection of Presidential Hats</t>
+  </si>
+  <si>
     <t>gadget_name</t>
   </si>
   <si>
     <t>gadget_desc</t>
+  </si>
+  <si>
+    <t>Riddler staff</t>
+  </si>
+  <si>
+    <t>Remote control unit for various gadgets</t>
+  </si>
+  <si>
+    <t>Tranqulizer gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An air rifle that fired darts tipped in sedative chemicals.</t>
+  </si>
+  <si>
+    <t>Instant Compound X</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A chemical meant to be used in conjunction with a plaster mask, after the latter has been adhered to a human face. The chemical creates a near-flawless mask mimicking the contours of that face.</t>
+  </si>
+  <si>
+    <t>Laughing Gas</t>
+  </si>
+  <si>
+    <t>Gas that induced uncontrollable laughter in those who breathed it without protection; extended exposure resulted in unconsciousness.</t>
+  </si>
+  <si>
+    <t>Super-Adhesive</t>
+  </si>
+  <si>
+    <t>A chemical spray that became incredibly sticky upon contact with air.</t>
+  </si>
+  <si>
+    <t>Explosives</t>
+  </si>
+  <si>
+    <t>Things that go boom.</t>
+  </si>
+  <si>
+    <t>Smoke-Bomb</t>
+  </si>
+  <si>
+    <t>Releases cloud of smoke intended to distract and diguise</t>
+  </si>
+  <si>
+    <t>Paraliyzing gas</t>
+  </si>
+  <si>
+    <t>Gas that renders victim immobile</t>
+  </si>
+  <si>
+    <t>Trick streamers</t>
+  </si>
+  <si>
+    <t>Ordinary-looking but unbreakable party streamers, usually deployed during battle to tie up enemies</t>
+  </si>
+  <si>
+    <t>Sneezing powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typical prank item that induced uncontrollable sneezing. Tended to be thrown in opponents' faces during battles as a distraction tactic.</t>
+  </si>
+  <si>
+    <t>Trick flower</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fake flower attached to the top buttonhole of a suit jacket; connected to a hose that allowed it to squirt water, knockout gas, etc.</t>
+  </si>
+  <si>
+    <t>Hand buzzer</t>
+  </si>
+  <si>
+    <t>Stuns targets when shaking hands</t>
+  </si>
+  <si>
+    <t>Umbrella gun</t>
+  </si>
+  <si>
+    <t>Firearm disguised as an ordinary umbrella</t>
+  </si>
+  <si>
+    <t>Gas umbrella</t>
+  </si>
+  <si>
+    <t>Umbrella used to dispense gasses (knock out, lauging, etc.)</t>
+  </si>
+  <si>
+    <t>Jetpack umbrella</t>
+  </si>
+  <si>
+    <t>Large umbrellas that allow the user to fly on top of them</t>
+  </si>
+  <si>
+    <t>Giant electro-magnet</t>
+  </si>
+  <si>
+    <t>A large magnet used to ensnare the Dynamic Duo by attracting the metal items in their utility belts</t>
+  </si>
+  <si>
+    <t>Bulletproof umbrella</t>
+  </si>
+  <si>
+    <t>Large umbrella that protects user from gun fire</t>
+  </si>
+  <si>
+    <t>Whip</t>
+  </si>
+  <si>
+    <t>Cat-o-nine-tails whip that dispenses deadly gas from the tips</t>
+  </si>
+  <si>
+    <t>See in the dark glasses</t>
+  </si>
+  <si>
+    <t>Glasses that allow the wearer to see in the dark</t>
+  </si>
+  <si>
+    <t>Voice-stealing box</t>
+  </si>
+  <si>
+    <t>A box that steals the voice of the person it is pointed at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catillac </t>
+  </si>
+  <si>
+    <t>Catwoman's primary mode of transportation</t>
+  </si>
+  <si>
+    <t>Tear gas eggs</t>
+  </si>
+  <si>
+    <t>Eggs laid by chickens on a diet of onions, release a gas that causes intense watering of the eyes</t>
+  </si>
+  <si>
+    <t>Freeze gun</t>
+  </si>
+  <si>
+    <t>Weapon that freezes targets, even entire rooms</t>
+  </si>
+  <si>
+    <t>Long bow</t>
+  </si>
+  <si>
+    <t>Standard bow that fires a range of novelty arrows</t>
+  </si>
+  <si>
+    <t>Rocket powered wheelchair</t>
+  </si>
+  <si>
+    <t>Super slick oil</t>
+  </si>
+  <si>
+    <t>Oil that can be spread on a floor or roadway to allow escape from pursuers</t>
+  </si>
+  <si>
+    <t>Super instant mesmerizer</t>
+  </si>
+  <si>
+    <t>Device concealed in a top hat that hypnotizes anyone that looks at it</t>
+  </si>
+  <si>
+    <t>Radio eyeglasses</t>
+  </si>
+  <si>
+    <t>Eyeglasses with hidden radio transmitter</t>
+  </si>
+  <si>
+    <t>gadget_id</t>
+  </si>
+  <si>
+    <t>crime_id</t>
   </si>
 </sst>
 </file>
@@ -381,6 +637,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1558,6 +1818,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="104.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1565,6 +1828,230 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="1">
+        <v>11.0</v>
       </c>
     </row>
   </sheetData>
@@ -1581,13 +2068,605 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.43"/>
+    <col customWidth="1" min="2" max="2" width="151.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>18.0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B28" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="B37" s="1">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="B41" s="1">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="B42" s="1">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="B43" s="1">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="B44" s="1">
+        <v>28.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>